<commit_message>
Adding novel ERV (Delta.9)
</commit_message>
<xml_diff>
--- a/tabular/erv/erv-refseqs-side-data.xlsx
+++ b/tabular/erv/erv-refseqs-side-data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/Retrovirus/Deltaretrovirus-GLUE/tabular/erv/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8153017-419E-884B-952C-81A5861F9E5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4D17AB-506C-0D47-A437-C7D676D3A89B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8080" yWindow="1540" windowWidth="40620" windowHeight="24600" xr2:uid="{BB705A9D-FBC1-AA49-AAF1-8BAD7726CAC1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="47">
   <si>
     <t>sequenceID</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>ERV-Delta.3-Murina_aurata</t>
+  </si>
+  <si>
+    <t>ERV-Delta.9-MolMol</t>
+  </si>
+  <si>
+    <t>ERV-Delta.9-Molossus_molossus</t>
+  </si>
+  <si>
+    <t>Molossus molossus</t>
   </si>
 </sst>
 </file>
@@ -546,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D3CDF3-D172-594F-9592-D3550A4BED8C}">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="B8" sqref="A1:K9"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -610,7 +619,7 @@
       <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E2" s="2" t="s">
@@ -645,7 +654,7 @@
       <c r="C3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E3" s="2" t="s">
@@ -680,7 +689,7 @@
       <c r="C4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -715,7 +724,7 @@
       <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="2" t="s">
@@ -750,7 +759,7 @@
       <c r="C6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -785,7 +794,7 @@
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="2" t="s">
         <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
@@ -820,7 +829,7 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -855,7 +864,7 @@
       <c r="C9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -877,6 +886,41 @@
         <v>27</v>
       </c>
       <c r="K9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" t="s">
+        <v>46</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>